<commit_message>
Added hash Sha256 or something
</commit_message>
<xml_diff>
--- a/Dokumenter/Filler/risikoAnalyse (2.xlsx
+++ b/Dokumenter/Filler/risikoAnalyse (2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/adbaa005_osloskolen_no/Documents/Videregående Skole/Vg2/IM/Biscuit Clicker 2.0/Dokumenter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/adbaa005_osloskolen_no/Documents/Videregående Skole/Vg2/IM/Biscuit Clicker 2.0/Dokumenter/Filler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{4666E808-344E-4EC7-ABFF-A9CFEE84FC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B591D808-6264-4E0B-BAA2-15DC2DDCEE6D}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{4666E808-344E-4EC7-ABFF-A9CFEE84FC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D373CCB3-531D-4887-922C-37099562448C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B79DEFEE-B3E0-4A78-B1D4-C3041B318B3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B79DEFEE-B3E0-4A78-B1D4-C3041B318B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Risiko analyse" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Risikoanalyse</t>
   </si>
@@ -108,84 +108,27 @@
     <t>Ansvarlig</t>
   </si>
   <si>
-    <t>Window 10 Pro</t>
-  </si>
-  <si>
-    <t>Desktop-erik4vn</t>
-  </si>
-  <si>
     <t>HP 260 Busniess PC</t>
   </si>
   <si>
-    <t>Brukernavn</t>
-  </si>
-  <si>
     <t>Passord</t>
   </si>
   <si>
     <t>Osloskolen</t>
   </si>
   <si>
-    <t>displayname</t>
-  </si>
-  <si>
-    <t>brukernavn</t>
-  </si>
-  <si>
-    <t>passord</t>
-  </si>
-  <si>
-    <t>dato</t>
-  </si>
-  <si>
-    <t>Ingen</t>
-  </si>
-  <si>
     <t>PHP</t>
   </si>
   <si>
-    <t>HTML</t>
-  </si>
-  <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
     <t>Bootstrap</t>
   </si>
   <si>
-    <t>Apache</t>
-  </si>
-  <si>
-    <t>Ubuntu</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>UFW</t>
-  </si>
-  <si>
-    <t>Ukentlig</t>
-  </si>
-  <si>
     <t>Nei</t>
   </si>
   <si>
-    <t>Windows Firewall</t>
-  </si>
-  <si>
-    <t>Unøyaktig</t>
-  </si>
-  <si>
     <t>10 Gbps CAT 6A</t>
   </si>
   <si>
-    <t>VPN site to site</t>
-  </si>
-  <si>
     <t>Systemintegritet - Utvikling</t>
   </si>
   <si>
@@ -228,41 +171,83 @@
     <t>Strømbrudd</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Håper på at Kuben har UPS</t>
   </si>
   <si>
     <t>Osloskolens Overvåknings System</t>
   </si>
   <si>
-    <t>Sikringer</t>
-  </si>
-  <si>
     <t>Oppdatering</t>
   </si>
   <si>
-    <t>Sikre kontoer</t>
-  </si>
-  <si>
-    <t>Ingen deling</t>
-  </si>
-  <si>
-    <t>Oppdatering/Få lært</t>
-  </si>
-  <si>
     <t>Meg</t>
   </si>
   <si>
     <t>Risikovurdering (15.01.2024)</t>
+  </si>
+  <si>
+    <t>Ext4</t>
+  </si>
+  <si>
+    <t>Daglig</t>
+  </si>
+  <si>
+    <t>Debian v.12</t>
+  </si>
+  <si>
+    <t>UFW (Uncomplicated firewall)</t>
+  </si>
+  <si>
+    <t>Brukernavn, Passord</t>
+  </si>
+  <si>
+    <t>displayname, brukernavn, passord og Dato</t>
+  </si>
+  <si>
+    <t>PHP, HTML, CSS, SQL, Apache, Debian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHA256 </t>
+  </si>
+  <si>
+    <t>Kryptere viktig data</t>
+  </si>
+  <si>
+    <t>Ingen nedlasting av ukjente elementer</t>
+  </si>
+  <si>
+    <t>Alltid bruke Bootstrap 5.3</t>
+  </si>
+  <si>
+    <t>Følge med på Oppdateringering</t>
+  </si>
+  <si>
+    <t>Ethernet</t>
+  </si>
+  <si>
+    <t>Alltid bruke PHP 8.3</t>
+  </si>
+  <si>
+    <t>Feilsøk og restart</t>
+  </si>
+  <si>
+    <t>Feilsøk brukere, rettigheter og nettverk</t>
+  </si>
+  <si>
+    <t>Konfigurer ufw</t>
+  </si>
+  <si>
+    <t>Sikre kabeller</t>
+  </si>
+  <si>
+    <t>Stabilt arbeidsmiljø</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,14 +331,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -395,7 +372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,7 +408,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Forklarende tekst" xfId="2" builtinId="53"/>
@@ -793,13 +775,13 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="2.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -834,158 +816,245 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
+      <c r="B9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
+      <c r="B10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
+      <c r="B11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="B13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
+      <c r="B14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
+      <c r="B15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
+      <c r="B19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="16">
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -997,7 +1066,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,14 +1075,14 @@
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" style="2"/>
-    <col min="5" max="5" width="30.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1044,7 +1113,7 @@
     </row>
     <row r="5" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
@@ -1056,15 +1125,15 @@
         <v>4</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
@@ -1076,15 +1145,15 @@
         <v>5</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7">
         <v>2</v>
@@ -1096,10 +1165,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
@@ -1116,18 +1185,18 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7">
         <v>4</v>
@@ -1136,15 +1205,15 @@
         <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
@@ -1156,35 +1225,35 @@
         <v>6</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B12" s="7">
         <v>3</v>
@@ -1196,15 +1265,15 @@
         <v>9</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B13" s="7">
         <v>2</v>
@@ -1216,15 +1285,15 @@
         <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
@@ -1236,15 +1305,15 @@
         <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7">
         <v>2</v>
@@ -1256,15 +1325,15 @@
         <v>8</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B16" s="7">
         <v>2</v>
@@ -1276,15 +1345,15 @@
         <v>10</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7">
         <v>1</v>
@@ -1296,15 +1365,15 @@
         <v>5</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7">
         <v>4</v>
@@ -1316,35 +1385,35 @@
         <v>16</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B19" s="7">
         <v>4</v>
       </c>
       <c r="C19" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="8">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B20" s="7">
         <v>4</v>
@@ -1356,31 +1425,16 @@
         <v>20</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="7">
-        <v>2</v>
-      </c>
-      <c r="C21" s="7">
-        <v>2</v>
-      </c>
-      <c r="D21" s="8">
-        <v>4</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>71</v>
-      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="D22" s="8"/>
@@ -1479,6 +1533,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="799c8709-ef66-4c6c-9db1-911ba3fb05c1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a6c765d7-93d9-4c2c-aec4-d1ca8eafcddb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100F08FE7F726CE83479C8ED4A0973BEC47" ma:contentTypeVersion="11" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="42a3d8d2653bf8369b837489e78664e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="799c8709-ef66-4c6c-9db1-911ba3fb05c1" xmlns:ns3="a6c765d7-93d9-4c2c-aec4-d1ca8eafcddb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0054c8493c321ce9feb586a6569ff8b" ns2:_="" ns3:_="">
     <xsd:import namespace="799c8709-ef66-4c6c-9db1-911ba3fb05c1"/>
@@ -1673,27 +1747,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D397892C-4107-4405-A41E-F7C43A9FB3B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27cd06e8-8e2b-4eab-b578-6ee18ff152a4"/>
+    <ds:schemaRef ds:uri="9a8bd0c8-94c0-4e76-bd03-7e285dab928e"/>
+    <ds:schemaRef ds:uri="799c8709-ef66-4c6c-9db1-911ba3fb05c1"/>
+    <ds:schemaRef ds:uri="a6c765d7-93d9-4c2c-aec4-d1ca8eafcddb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="799c8709-ef66-4c6c-9db1-911ba3fb05c1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a6c765d7-93d9-4c2c-aec4-d1ca8eafcddb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E69B3A1-1CC0-4B83-BCBA-02417EAE80CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A7F273C-7402-4B3E-9954-0673656DD6A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1710,25 +1785,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E69B3A1-1CC0-4B83-BCBA-02417EAE80CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D397892C-4107-4405-A41E-F7C43A9FB3B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27cd06e8-8e2b-4eab-b578-6ee18ff152a4"/>
-    <ds:schemaRef ds:uri="9a8bd0c8-94c0-4e76-bd03-7e285dab928e"/>
-    <ds:schemaRef ds:uri="799c8709-ef66-4c6c-9db1-911ba3fb05c1"/>
-    <ds:schemaRef ds:uri="a6c765d7-93d9-4c2c-aec4-d1ca8eafcddb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>